<commit_message>
AoC 2024 - Excel update
</commit_message>
<xml_diff>
--- a/2024/Exploration.xlsx
+++ b/2024/Exploration.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Nucular\AdventOfCode\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8EFE7E-37A3-4871-80A7-34E092084AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB498CC-BBAA-4F18-A551-6800C9ADCC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5BCDD9EA-4D95-46EA-9524-FDF4489961B0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{5BCDD9EA-4D95-46EA-9524-FDF4489961B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Dayz" sheetId="4" r:id="rId1"/>
     <sheet name="Day 11" sheetId="1" r:id="rId2"/>
     <sheet name="Day 13 - Part I" sheetId="2" r:id="rId3"/>
     <sheet name="Day 17" sheetId="3" r:id="rId4"/>
+    <sheet name="Day 20" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="56">
   <si>
     <t>X</t>
   </si>
@@ -187,6 +188,15 @@
   </si>
   <si>
     <t>Don't know the solution</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -603,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A415CB80-8396-44D9-A08C-E57C52E9FE9D}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1716,4 +1726,68 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D129BC4-970A-4A2F-B1D6-F7951F6186FA}">
+  <dimension ref="B3:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="3" spans="2:6">
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AoC 2024 - Day 24 (solution, part I)
</commit_message>
<xml_diff>
--- a/2024/Exploration.xlsx
+++ b/2024/Exploration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Nucular\AdventOfCode\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB498CC-BBAA-4F18-A551-6800C9ADCC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553D2A97-47A5-43B5-A37B-52E34C4B26D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{5BCDD9EA-4D95-46EA-9524-FDF4489961B0}"/>
+    <workbookView xWindow="28635" yWindow="-165" windowWidth="29130" windowHeight="15810" activeTab="5" xr2:uid="{5BCDD9EA-4D95-46EA-9524-FDF4489961B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Dayz" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Day 13 - Part I" sheetId="2" r:id="rId3"/>
     <sheet name="Day 17" sheetId="3" r:id="rId4"/>
     <sheet name="Day 20" sheetId="5" r:id="rId5"/>
+    <sheet name="Day 24" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="63">
   <si>
     <t>X</t>
   </si>
@@ -197,6 +198,27 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>--&gt;</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>XOR</t>
+  </si>
+  <si>
+    <t>AND</t>
   </si>
 </sst>
 </file>
@@ -1732,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D129BC4-970A-4A2F-B1D6-F7951F6186FA}">
   <dimension ref="B3:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -1790,4 +1812,171 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB3AC13-BF3F-46B3-A564-206156AC5828}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>